<commit_message>
Closing April Month and forcast May 2025
</commit_message>
<xml_diff>
--- a/Monthly_Cost_For_APR_2025.xlsx
+++ b/Monthly_Cost_For_APR_2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G177"/>
+  <dimension ref="A1:G180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.0115229662</v>
+        <v>0.018310198</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.9914217846</v>
+        <v>2.2583540171</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>93.7334960825</v>
+        <v>201.9561796567</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.24</v>
+        <v>0.44</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>1903.2875905749</v>
+        <v>3862.658378276</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1141.12</v>
+        <v>2427.485</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>6.18</v>
+        <v>22.31</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>6.1958573827</v>
+        <v>14.6930867961</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>1586.4635000226</v>
+        <v>3369.8865002243</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>154.4973666516</v>
+        <v>328.135999968</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>246.4204946555</v>
+        <v>525.5472072854</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -987,7 +987,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>13.56</v>
+        <v>28.8</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>8.95776e-05</v>
+        <v>0.000191952</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1.4125000113</v>
+        <v>3.000000024</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>16.95</v>
+        <v>36</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1127,7 +1127,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>0.913</v>
+        <v>1.8399106</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>80.5534846032</v>
+        <v>169.9781978363</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>0.9518523408</v>
+        <v>2.0330995715</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0.4685265593</v>
+        <v>0.9982302302</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1267,7 +1267,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>0.4715863371</v>
+        <v>1.0002461191</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>32.9350290233</v>
+        <v>70.3806495092</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>30.1188333716</v>
+        <v>64.3410242078</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>0.9361111186</v>
+        <v>1.9944444604</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1407,7 +1407,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>0.4685265593</v>
+        <v>0.9982302302</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>961.4293373329</v>
+        <v>1947.3642022206</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1477,7 +1477,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>5.0373713335</v>
+        <v>10.5034207646</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>16.6613893526</v>
+        <v>26.3289988771</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1547,11 +1547,11 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>0.4197824222</v>
+        <v>0.002509905</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$aardvark-prd</t>
         </is>
       </c>
     </row>
@@ -1582,11 +1582,11 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>1.096949739</v>
+        <v>0.8922328279</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -1617,11 +1617,11 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>2.8510678399</v>
+        <v>2.2316960866</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -1652,11 +1652,11 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>7.7029531415</v>
+        <v>6.08734491</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -1687,11 +1687,11 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>0.3586201011</v>
+        <v>16.596673049</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -1718,15 +1718,15 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>AWS Secrets Manager</t>
+          <t>AWS Lambda</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>66.79691715449999</v>
+        <v>0.7632345961</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -1757,11 +1757,11 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>40.90894</v>
+        <v>139.9620049202</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -1792,11 +1792,11 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>20.08001</v>
+        <v>4e-05</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -1823,15 +1823,15 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>AWS Security Hub</t>
+          <t>AWS Secrets Manager</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>132.15861</v>
+        <v>79.99590999999999</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -1858,15 +1858,15 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>AWS Step Functions</t>
+          <t>AWS Secrets Manager</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>0.0012125516</v>
+        <v>43.34476</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -1893,11 +1893,11 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>AWS Support (Enterprise)</t>
+          <t>AWS Security Hub</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>27285.49</v>
+        <v>256.28941</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
@@ -1928,11 +1928,11 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>AWS Systems Manager</t>
+          <t>AWS Step Functions</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>0.07119</v>
+        <v>0.0025753843</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -1963,11 +1963,11 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>AWS Transfer Family</t>
+          <t>AWS Support (Enterprise)</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>101.9408533679</v>
+        <v>45349.55</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -1998,11 +1998,11 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>AWS WAF</t>
+          <t>AWS Systems Manager</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>55.7044874689</v>
+        <v>0.1512</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
@@ -2033,15 +2033,15 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>AWS WAF</t>
+          <t>AWS Transfer Family</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>5.7672260742</v>
+        <v>216.5989560527</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2072,11 +2072,11 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>754.4052266742</v>
+        <v>117.2308714544</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2103,15 +2103,15 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>AWS X-Ray</t>
+          <t>AWS WAF</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>24.725177</v>
+        <v>12.395795016</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2138,15 +2138,15 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Amazon API Gateway</t>
+          <t>AWS WAF</t>
         </is>
       </c>
       <c r="F49" t="n">
-        <v>139.014502324</v>
+        <v>1607.129184216</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2173,11 +2173,11 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Amazon Athena</t>
+          <t>AWS X-Ray</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>5.652765</v>
+        <v>55.325243</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -2208,11 +2208,11 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Amazon CloudFront</t>
+          <t>Amazon API Gateway</t>
         </is>
       </c>
       <c r="F51" t="n">
-        <v>7627.1258096222</v>
+        <v>313.5993615689</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -2243,15 +2243,15 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Amazon CloudFront</t>
+          <t>Amazon Athena</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>0.7067241338</v>
+        <v>12.97906</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2282,11 +2282,11 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>0.9663669341</v>
+        <v>16589.242359253</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2317,11 +2317,11 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>2583.4511531381</v>
+        <v>1.8166019233</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2352,11 +2352,11 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>0.0216865902</v>
+        <v>1.941728243</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Environment$qa</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -2387,11 +2387,11 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>4.741e-07</v>
+        <v>5603.5864722339</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2418,15 +2418,15 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Amazon Cognito</t>
+          <t>Amazon CloudFront</t>
         </is>
       </c>
       <c r="F57" t="n">
-        <v>85.13500000000001</v>
+        <v>0.0750319845</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$qa</t>
         </is>
       </c>
     </row>
@@ -2453,15 +2453,15 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Amazon Detective</t>
+          <t>Amazon CloudFront</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>63.5086428358</v>
+        <v>1.0886e-06</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -2488,11 +2488,11 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Amazon DevOps Guru</t>
+          <t>Amazon Cognito</t>
         </is>
       </c>
       <c r="F59" t="n">
-        <v>0</v>
+        <v>98.16500000000001</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2523,11 +2523,11 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Amazon DocumentDB (with MongoDB compatibility)</t>
+          <t>Amazon Detective</t>
         </is>
       </c>
       <c r="F60" t="n">
-        <v>0.0742075351</v>
+        <v>126.3661110938</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2558,15 +2558,15 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Amazon DocumentDB (with MongoDB compatibility)</t>
+          <t>Amazon DevOps Guru</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>124.919298048</v>
+        <v>0</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2597,11 +2597,11 @@
         </is>
       </c>
       <c r="F62" t="n">
-        <v>139.254755245</v>
+        <v>0.160035912</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2628,15 +2628,15 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Amazon DynamoDB</t>
+          <t>Amazon DocumentDB (with MongoDB compatibility)</t>
         </is>
       </c>
       <c r="F63" t="n">
-        <v>22.6788330977</v>
+        <v>267.3744874166</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2663,15 +2663,15 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Amazon DynamoDB</t>
+          <t>Amazon DocumentDB (with MongoDB compatibility)</t>
         </is>
       </c>
       <c r="F64" t="n">
-        <v>26.9022992454</v>
+        <v>250.3805634179</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2702,11 +2702,11 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>58.5741930115</v>
+        <v>73.23719882659999</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2733,15 +2733,15 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Amazon EC2 Container Registry (ECR)</t>
+          <t>Amazon DynamoDB</t>
         </is>
       </c>
       <c r="F66" t="n">
-        <v>61.6708163988</v>
+        <v>36.5652019185</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2768,15 +2768,15 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Amazon EC2 Container Registry (ECR)</t>
+          <t>Amazon DynamoDB</t>
         </is>
       </c>
       <c r="F67" t="n">
-        <v>0.0172365906</v>
+        <v>126.2439047233</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Environment$common</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2807,11 +2807,11 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>0.189284718</v>
+        <v>131.2250778855</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2842,11 +2842,11 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>403.0111851258</v>
+        <v>0.036608688</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$common</t>
         </is>
       </c>
     </row>
@@ -2873,15 +2873,15 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Amazon ElastiCache</t>
+          <t>Amazon EC2 Container Registry (ECR)</t>
         </is>
       </c>
       <c r="F70" t="n">
-        <v>7001.6921815128</v>
+        <v>0.40202064</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -2908,15 +2908,15 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Amazon ElastiCache</t>
+          <t>Amazon EC2 Container Registry (ECR)</t>
         </is>
       </c>
       <c r="F71" t="n">
-        <v>3140.499182625</v>
+        <v>861.9272326576</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -2947,11 +2947,11 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>2538.432</v>
+        <v>11012.7087344036</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -2978,15 +2978,15 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>EC2 - Other</t>
+          <t>Amazon ElastiCache</t>
         </is>
       </c>
       <c r="F73" t="n">
-        <v>11311.8463093855</v>
+        <v>6653.917992423</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3013,15 +3013,15 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>EC2 - Other</t>
+          <t>Amazon ElastiCache</t>
         </is>
       </c>
       <c r="F74" t="n">
-        <v>0.3699999963</v>
+        <v>5391.36</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Environment$PSFalcon</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3052,11 +3052,11 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>0.8099034998</v>
+        <v>24013.3944175255</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3087,11 +3087,11 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>9.2777777852</v>
+        <v>0.799999992</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Environment$management</t>
+          <t>Environment$PSFalcon</t>
         </is>
       </c>
     </row>
@@ -3122,11 +3122,11 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>528.6713304208</v>
+        <v>1.8038082853</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -3157,11 +3157,11 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>8.776708666499999</v>
+        <v>20.000000016</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$management</t>
         </is>
       </c>
     </row>
@@ -3192,11 +3192,11 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>3685.5604845128</v>
+        <v>1177.3104398748</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3227,11 +3227,11 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>0.3827064288</v>
+        <v>20.2332074584</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -3258,15 +3258,15 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Amazon Elastic Compute Cloud - Compute</t>
+          <t>EC2 - Other</t>
         </is>
       </c>
       <c r="F81" t="n">
-        <v>10287.7760281411</v>
+        <v>7546.4936633632</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3293,15 +3293,15 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Amazon Elastic Compute Cloud - Compute</t>
+          <t>EC2 - Other</t>
         </is>
       </c>
       <c r="F82" t="n">
-        <v>29.2032</v>
+        <v>0.8688794697</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -3332,11 +3332,11 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>3702.9810912905</v>
+        <v>20088.5403112081</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3367,11 +3367,11 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>47.0385413024</v>
+        <v>62.208</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -3402,11 +3402,11 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>31777.3073336838</v>
+        <v>7752.8203793013</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3437,11 +3437,11 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>29.14716773</v>
+        <v>56.6433413024</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -3468,15 +3468,15 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Amazon Elastic Container Service</t>
+          <t>Amazon Elastic Compute Cloud - Compute</t>
         </is>
       </c>
       <c r="F87" t="n">
-        <v>4749.5096214763</v>
+        <v>68445.8188727933</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3503,15 +3503,15 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Amazon Elastic Container Service for Kubernetes</t>
+          <t>Amazon Elastic Compute Cloud - Compute</t>
         </is>
       </c>
       <c r="F88" t="n">
-        <v>259.3888895749</v>
+        <v>35.199799914</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -3538,15 +3538,15 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Amazon Elastic Container Service for Kubernetes</t>
+          <t>Amazon Elastic Container Service</t>
         </is>
       </c>
       <c r="F89" t="n">
-        <v>271.2</v>
+        <v>8595.0887986295</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3577,11 +3577,11 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>305.1</v>
+        <v>550.6678597435</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3608,15 +3608,15 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Amazon Elastic File System</t>
+          <t>Amazon Elastic Container Service for Kubernetes</t>
         </is>
       </c>
       <c r="F91" t="n">
-        <v>37.0956650739</v>
+        <v>576</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3643,15 +3643,15 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Amazon Elastic Load Balancing</t>
+          <t>Amazon Elastic Container Service for Kubernetes</t>
         </is>
       </c>
       <c r="F92" t="n">
-        <v>3705.538040288</v>
+        <v>648</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3678,15 +3678,15 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Amazon Elastic Load Balancing</t>
+          <t>Amazon Elastic File System</t>
         </is>
       </c>
       <c r="F93" t="n">
-        <v>7.6276130286</v>
+        <v>78.7876735258</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3717,11 +3717,11 @@
         </is>
       </c>
       <c r="F94" t="n">
-        <v>7.8061991642</v>
+        <v>7585.5920242904</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -3752,11 +3752,11 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>138.2116295961</v>
+        <v>16.200239709</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -3787,11 +3787,11 @@
         </is>
       </c>
       <c r="F96" t="n">
-        <v>22.8889149346</v>
+        <v>16.4714127525</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -3822,11 +3822,11 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>1060.6994035221</v>
+        <v>304.6317003922</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -3857,11 +3857,11 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>7.6766644541</v>
+        <v>48.6129167567</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -3888,15 +3888,15 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Amazon Glacier</t>
+          <t>Amazon Elastic Load Balancing</t>
         </is>
       </c>
       <c r="F99" t="n">
-        <v>1.2043652936</v>
+        <v>2207.8013229619</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -3923,15 +3923,15 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Amazon GuardDuty</t>
+          <t>Amazon Elastic Load Balancing</t>
         </is>
       </c>
       <c r="F100" t="n">
-        <v>1965.0187747143</v>
+        <v>16.2977127262</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -3958,11 +3958,11 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Amazon Inspector</t>
+          <t>Amazon Glacier</t>
         </is>
       </c>
       <c r="F101" t="n">
-        <v>1.2</v>
+        <v>2.5807818608</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
@@ -3993,11 +3993,11 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Amazon Kinesis</t>
+          <t>Amazon GuardDuty</t>
         </is>
       </c>
       <c r="F102" t="n">
-        <v>50.85</v>
+        <v>3593.2134394658</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -4028,11 +4028,11 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Amazon Lightsail</t>
+          <t>Amazon Inspector</t>
         </is>
       </c>
       <c r="F103" t="n">
-        <v>4.6826096528</v>
+        <v>2.4</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
@@ -4063,11 +4063,11 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Amazon Location Service</t>
+          <t>Amazon Kinesis</t>
         </is>
       </c>
       <c r="F104" t="n">
-        <v>0.0011355</v>
+        <v>108</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
@@ -4098,11 +4098,11 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Amazon MQ</t>
+          <t>Amazon Lightsail</t>
         </is>
       </c>
       <c r="F105" t="n">
-        <v>30.4715337614</v>
+        <v>9.9593802268</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
@@ -4133,15 +4133,15 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Amazon MQ</t>
+          <t>Amazon Location Service</t>
         </is>
       </c>
       <c r="F106" t="n">
-        <v>107.0092656574</v>
+        <v>0.002341</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4172,11 +4172,11 @@
         </is>
       </c>
       <c r="F107" t="n">
-        <v>110.4731381716</v>
+        <v>64.7196129182</v>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4203,15 +4203,15 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Amazon Macie</t>
+          <t>Amazon MQ</t>
         </is>
       </c>
       <c r="F108" t="n">
-        <v>1.1508</v>
+        <v>227.2173352906</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -4238,15 +4238,15 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Amazon Managed Grafana</t>
+          <t>Amazon MQ</t>
         </is>
       </c>
       <c r="F109" t="n">
-        <v>9</v>
+        <v>230.6999185604</v>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -4273,11 +4273,11 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Amazon Managed Workflows for Apache Airflow</t>
+          <t>Amazon Macie</t>
         </is>
       </c>
       <c r="F110" t="n">
-        <v>4176.1267025852</v>
+        <v>2.466</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
@@ -4308,15 +4308,15 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Amazon Managed Workflows for Apache Airflow</t>
+          <t>Amazon Managed Grafana</t>
         </is>
       </c>
       <c r="F111" t="n">
-        <v>1339.3912020786</v>
+        <v>9</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4347,11 +4347,11 @@
         </is>
       </c>
       <c r="F112" t="n">
-        <v>1339.6348075176</v>
+        <v>8724.757408136</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4378,15 +4378,15 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Amazon Neptune</t>
+          <t>Amazon Managed Workflows for Apache Airflow</t>
         </is>
       </c>
       <c r="F113" t="n">
-        <v>2.2182282708</v>
+        <v>2810.4642038484</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -4413,15 +4413,15 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Amazon OpenSearch Service</t>
+          <t>Amazon Managed Workflows for Apache Airflow</t>
         </is>
       </c>
       <c r="F114" t="n">
-        <v>407.733195335</v>
+        <v>2848.3948075176</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -4448,15 +4448,15 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Amazon OpenSearch Service</t>
+          <t>Amazon Neptune</t>
         </is>
       </c>
       <c r="F115" t="n">
-        <v>5151.6083742599</v>
+        <v>4.8339602162</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4487,11 +4487,11 @@
         </is>
       </c>
       <c r="F116" t="n">
-        <v>14664.7176819995</v>
+        <v>719.7938085717</v>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4518,15 +4518,15 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Amazon Personalize</t>
+          <t>Amazon OpenSearch Service</t>
         </is>
       </c>
       <c r="F117" t="n">
-        <v>323.396766</v>
+        <v>10486.2298930081</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -4553,15 +4553,15 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Amazon Polly</t>
+          <t>Amazon OpenSearch Service</t>
         </is>
       </c>
       <c r="F118" t="n">
-        <v>0.12556</v>
+        <v>30650.1828089863</v>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -4588,11 +4588,11 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Amazon QuickSight</t>
+          <t>Amazon Personalize</t>
         </is>
       </c>
       <c r="F119" t="n">
-        <v>30.0952891638</v>
+        <v>628.193718</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
@@ -4623,11 +4623,11 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Amazon Redshift</t>
+          <t>Amazon Polly</t>
         </is>
       </c>
       <c r="F120" t="n">
-        <v>191.385016944</v>
+        <v>0.12556</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
@@ -4658,11 +4658,11 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Amazon Relational Database Service</t>
+          <t>Amazon QuickSight</t>
         </is>
       </c>
       <c r="F121" t="n">
-        <v>37145.3316709292</v>
+        <v>63.9208701426</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
@@ -4693,15 +4693,15 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Amazon Relational Database Service</t>
+          <t>Amazon Redshift</t>
         </is>
       </c>
       <c r="F122" t="n">
-        <v>0.0008106535</v>
+        <v>406.45043762</v>
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>Environment$loadtest</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4732,11 +4732,11 @@
         </is>
       </c>
       <c r="F123" t="n">
-        <v>1857.698872506</v>
+        <v>68736.7160451355</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4767,11 +4767,11 @@
         </is>
       </c>
       <c r="F124" t="n">
-        <v>5769.4078017605</v>
+        <v>0.00173196</v>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$loadtest</t>
         </is>
       </c>
     </row>
@@ -4798,15 +4798,15 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Amazon Route 53</t>
+          <t>Amazon Relational Database Service</t>
         </is>
       </c>
       <c r="F125" t="n">
-        <v>981.2344141118</v>
+        <v>3762.5829561782</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -4833,15 +4833,15 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Amazon Route 53</t>
+          <t>Amazon Relational Database Service</t>
         </is>
       </c>
       <c r="F126" t="n">
-        <v>0.1576906</v>
+        <v>11648.9241565445</v>
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>Environment$Dev</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -4872,11 +4872,11 @@
         </is>
       </c>
       <c r="F127" t="n">
-        <v>0.1</v>
+        <v>1757.9963815907</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -4907,11 +4907,11 @@
         </is>
       </c>
       <c r="F128" t="n">
-        <v>0.1</v>
+        <v>0.1989662</v>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>Environment$common</t>
+          <t>Environment$Dev</t>
         </is>
       </c>
     </row>
@@ -4942,11 +4942,11 @@
         </is>
       </c>
       <c r="F129" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>Environment$global</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -4977,11 +4977,11 @@
         </is>
       </c>
       <c r="F130" t="n">
-        <v>0.1001532</v>
+        <v>0.1</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>Environment$loadtest</t>
+          <t>Environment$common</t>
         </is>
       </c>
     </row>
@@ -5012,11 +5012,11 @@
         </is>
       </c>
       <c r="F131" t="n">
-        <v>14.4859338</v>
+        <v>0.5</v>
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$global</t>
         </is>
       </c>
     </row>
@@ -5047,11 +5047,11 @@
         </is>
       </c>
       <c r="F132" t="n">
-        <v>8.1394454</v>
+        <v>0.1002594</v>
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$loadtest</t>
         </is>
       </c>
     </row>
@@ -5082,11 +5082,11 @@
         </is>
       </c>
       <c r="F133" t="n">
-        <v>0.1001292</v>
+        <v>16.1093794</v>
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>Environment$sandbox</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -5117,11 +5117,11 @@
         </is>
       </c>
       <c r="F134" t="n">
-        <v>0.1000138</v>
+        <v>12.7924294</v>
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -5152,11 +5152,11 @@
         </is>
       </c>
       <c r="F135" t="n">
-        <v>0.1</v>
+        <v>0.1002242</v>
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>Environment$test</t>
+          <t>Environment$sandbox</t>
         </is>
       </c>
     </row>
@@ -5183,15 +5183,15 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Amazon SageMaker</t>
+          <t>Amazon Route 53</t>
         </is>
       </c>
       <c r="F136" t="n">
-        <v>1030.8927958728</v>
+        <v>0.10002</v>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -5218,15 +5218,15 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Amazon Simple Email Service</t>
+          <t>Amazon Route 53</t>
         </is>
       </c>
       <c r="F137" t="n">
-        <v>6.2585195505</v>
+        <v>0.1</v>
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$test</t>
         </is>
       </c>
     </row>
@@ -5253,11 +5253,11 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Amazon Simple Notification Service</t>
+          <t>Amazon SageMaker</t>
         </is>
       </c>
       <c r="F138" t="n">
-        <v>8.052647737999999</v>
+        <v>1689.2164875133</v>
       </c>
       <c r="G138" t="inlineStr">
         <is>
@@ -5288,15 +5288,15 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Amazon Simple Notification Service</t>
+          <t>Amazon Simple Email Service</t>
         </is>
       </c>
       <c r="F139" t="n">
-        <v>0.0028156711</v>
+        <v>13.4987391481</v>
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>Environment$Common</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5327,11 +5327,11 @@
         </is>
       </c>
       <c r="F140" t="n">
-        <v>2.7e-05</v>
+        <v>17.6962371036</v>
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5362,11 +5362,11 @@
         </is>
       </c>
       <c r="F141" t="n">
-        <v>3.5e-06</v>
+        <v>0.0067967359</v>
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>Environment$Sandbox</t>
+          <t>Environment$Common</t>
         </is>
       </c>
     </row>
@@ -5397,11 +5397,11 @@
         </is>
       </c>
       <c r="F142" t="n">
-        <v>2.75e-05</v>
+        <v>6e-05</v>
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -5428,15 +5428,15 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Amazon Simple Queue Service</t>
+          <t>Amazon Simple Notification Service</t>
         </is>
       </c>
       <c r="F143" t="n">
-        <v>15.825852187</v>
+        <v>7.5e-06</v>
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$Sandbox</t>
         </is>
       </c>
     </row>
@@ -5463,15 +5463,15 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Amazon Simple Queue Service</t>
+          <t>Amazon Simple Notification Service</t>
         </is>
       </c>
       <c r="F144" t="n">
-        <v>4.92e-05</v>
+        <v>5.95e-05</v>
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -5502,11 +5502,11 @@
         </is>
       </c>
       <c r="F145" t="n">
-        <v>0.5744470508</v>
+        <v>33.1994066771</v>
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5537,11 +5537,11 @@
         </is>
       </c>
       <c r="F146" t="n">
-        <v>0.7232240532</v>
+        <v>0.0001036</v>
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -5568,15 +5568,15 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>Amazon Simple Storage Service</t>
+          <t>Amazon Simple Queue Service</t>
         </is>
       </c>
       <c r="F147" t="n">
-        <v>16909.9388797114</v>
+        <v>1.243480905</v>
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -5603,15 +5603,15 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>Amazon Simple Storage Service</t>
+          <t>Amazon Simple Queue Service</t>
         </is>
       </c>
       <c r="F148" t="n">
-        <v>0.0346426646</v>
+        <v>1.5481579113</v>
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>Environment$Common</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -5642,11 +5642,11 @@
         </is>
       </c>
       <c r="F149" t="n">
-        <v>0.0001169523</v>
+        <v>35546.4429553807</v>
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>Environment$Dev</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -5677,11 +5677,11 @@
         </is>
       </c>
       <c r="F150" t="n">
-        <v>0.0394132317</v>
+        <v>0.0739974019</v>
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>Environment$POC</t>
+          <t>Environment$Common</t>
         </is>
       </c>
     </row>
@@ -5712,11 +5712,11 @@
         </is>
       </c>
       <c r="F151" t="n">
-        <v>0.0176520694</v>
+        <v>0.0002491735</v>
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>Environment$Production</t>
+          <t>Environment$Dev</t>
         </is>
       </c>
     </row>
@@ -5747,11 +5747,11 @@
         </is>
       </c>
       <c r="F152" t="n">
-        <v>0.0004702208</v>
+        <v>0.0828904196</v>
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>Environment$Sandbox</t>
+          <t>Environment$POC</t>
         </is>
       </c>
     </row>
@@ -5782,11 +5782,11 @@
         </is>
       </c>
       <c r="F153" t="n">
-        <v>0.0012518502</v>
+        <v>0.0383694669</v>
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>Environment$common</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -5817,11 +5817,11 @@
         </is>
       </c>
       <c r="F154" t="n">
-        <v>10.8303782681</v>
+        <v>0.0009619512</v>
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>Environment$dev</t>
+          <t>Environment$Sandbox</t>
         </is>
       </c>
     </row>
@@ -5852,11 +5852,11 @@
         </is>
       </c>
       <c r="F155" t="n">
-        <v>0.0474402738</v>
+        <v>0.0026477281</v>
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>Environment$loadtest</t>
+          <t>Environment$common</t>
         </is>
       </c>
     </row>
@@ -5887,11 +5887,11 @@
         </is>
       </c>
       <c r="F156" t="n">
-        <v>815.4560350999</v>
+        <v>22.7615946556</v>
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$dev</t>
         </is>
       </c>
     </row>
@@ -5922,11 +5922,11 @@
         </is>
       </c>
       <c r="F157" t="n">
-        <v>1.6998522494</v>
+        <v>0.1019668793</v>
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$loadtest</t>
         </is>
       </c>
     </row>
@@ -5957,11 +5957,11 @@
         </is>
       </c>
       <c r="F158" t="n">
-        <v>8852.0033332108</v>
+        <v>1703.3301135673</v>
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -5992,11 +5992,11 @@
         </is>
       </c>
       <c r="F159" t="n">
-        <v>0.000407295</v>
+        <v>3.53198063</v>
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>Environment$qa</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -6027,11 +6027,11 @@
         </is>
       </c>
       <c r="F160" t="n">
-        <v>0.0016024013</v>
+        <v>18587.3880031316</v>
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>Environment$stg</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -6058,15 +6058,15 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>Amazon Simple Workflow Service</t>
+          <t>Amazon Simple Storage Service</t>
         </is>
       </c>
       <c r="F161" t="n">
-        <v>5.1e-07</v>
+        <v>0.000883475</v>
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$qa</t>
         </is>
       </c>
     </row>
@@ -6093,15 +6093,15 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Amazon SimpleDB</t>
+          <t>Amazon Simple Storage Service</t>
         </is>
       </c>
       <c r="F162" t="n">
-        <v>6.2833e-06</v>
+        <v>0.0035631691</v>
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$stg</t>
         </is>
       </c>
     </row>
@@ -6128,11 +6128,11 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>Amazon Virtual Private Cloud</t>
+          <t>Amazon Simple Workflow Service</t>
         </is>
       </c>
       <c r="F163" t="n">
-        <v>4741.8551684743</v>
+        <v>9.138e-07</v>
       </c>
       <c r="G163" t="inlineStr">
         <is>
@@ -6163,15 +6163,15 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>Amazon Virtual Private Cloud</t>
+          <t>Amazon SimpleDB</t>
         </is>
       </c>
       <c r="F164" t="n">
-        <v>73.62</v>
+        <v>1.12207e-05</v>
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -6202,11 +6202,11 @@
         </is>
       </c>
       <c r="F165" t="n">
-        <v>1.68</v>
+        <v>9810.011010471801</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>Environment$prd</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -6237,11 +6237,11 @@
         </is>
       </c>
       <c r="F166" t="n">
-        <v>71.1400336849</v>
+        <v>8.3335e-05</v>
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$Production</t>
         </is>
       </c>
     </row>
@@ -6272,11 +6272,11 @@
         </is>
       </c>
       <c r="F167" t="n">
-        <v>46.1287981012</v>
+        <v>155.72</v>
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>Environment$shared</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -6303,15 +6303,15 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>Amazon WorkSpaces</t>
+          <t>Amazon Virtual Private Cloud</t>
         </is>
       </c>
       <c r="F168" t="n">
-        <v>19</v>
+        <v>3.6</v>
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prd</t>
         </is>
       </c>
     </row>
@@ -6338,15 +6338,15 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>AmazonCloudWatch</t>
+          <t>Amazon Virtual Private Cloud</t>
         </is>
       </c>
       <c r="F169" t="n">
-        <v>6427.4051825463</v>
+        <v>151.2000336849</v>
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -6373,15 +6373,15 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>AmazonCloudWatch</t>
+          <t>Amazon Virtual Private Cloud</t>
         </is>
       </c>
       <c r="F170" t="n">
-        <v>408.8405061498</v>
+        <v>97.8751743664</v>
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>Environment$nonprod</t>
+          <t>Environment$shared</t>
         </is>
       </c>
     </row>
@@ -6408,15 +6408,15 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>AmazonCloudWatch</t>
+          <t>Amazon WorkSpaces</t>
         </is>
       </c>
       <c r="F171" t="n">
-        <v>2289.4595113989</v>
+        <v>19.68</v>
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>Environment$prod</t>
+          <t>Environment$</t>
         </is>
       </c>
     </row>
@@ -6443,11 +6443,11 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>AmazonWorkMail</t>
+          <t>AmazonCloudWatch</t>
         </is>
       </c>
       <c r="F172" t="n">
-        <v>92.283333258</v>
+        <v>12916.3464565488</v>
       </c>
       <c r="G172" t="inlineStr">
         <is>
@@ -6478,15 +6478,15 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>CloudWatch Events</t>
+          <t>AmazonCloudWatch</t>
         </is>
       </c>
       <c r="F173" t="n">
-        <v>2.7131536003</v>
+        <v>871.6689104685</v>
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$nonprod</t>
         </is>
       </c>
     </row>
@@ -6513,15 +6513,15 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>CrowdStrike Falcon Endpoint Protection</t>
+          <t>AmazonCloudWatch</t>
         </is>
       </c>
       <c r="F174" t="n">
-        <v>76531.06</v>
+        <v>4799.655904202</v>
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>Environment$</t>
+          <t>Environment$prod</t>
         </is>
       </c>
     </row>
@@ -6548,11 +6548,11 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>Savings Plans for AWS Compute usage</t>
+          <t>AmazonWorkMail</t>
         </is>
       </c>
       <c r="F175" t="n">
-        <v>28800</v>
+        <v>195.99999984</v>
       </c>
       <c r="G175" t="inlineStr">
         <is>
@@ -6583,11 +6583,11 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>Tax</t>
+          <t>CloudWatch Events</t>
         </is>
       </c>
       <c r="F176" t="n">
-        <v>12090.89</v>
+        <v>4.1240101512</v>
       </c>
       <c r="G176" t="inlineStr">
         <is>
@@ -6618,13 +6618,118 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
+          <t>CrowdStrike Falcon Endpoint Protection</t>
+        </is>
+      </c>
+      <c r="F177" t="n">
+        <v>76531.06</v>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>Environment$</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>APR</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Entercom Communications</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>724972922289</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>Savings Plans for AWS Compute usage</t>
+        </is>
+      </c>
+      <c r="F178" t="n">
+        <v>28800</v>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>Environment$</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>APR</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Entercom Communications</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>724972922289</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>Tax</t>
+        </is>
+      </c>
+      <c r="F179" t="n">
+        <v>17028.18</v>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>Environment$</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>APR</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Entercom Communications</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>724972922289</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
           <t>Upwind Runtime-Powered Cloud Security Platform</t>
         </is>
       </c>
-      <c r="F177" t="n">
+      <c r="F180" t="n">
         <v>48000</v>
       </c>
-      <c r="G177" t="inlineStr">
+      <c r="G180" t="inlineStr">
         <is>
           <t>Environment$</t>
         </is>

</xml_diff>